<commit_message>
Added charge per appt
</commit_message>
<xml_diff>
--- a/src/Samples/AppartementDetails.xlsx
+++ b/src/Samples/AppartementDetails.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\invoice-generator\src\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\invoice-generator\src\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2899A7-132D-4087-9C94-1A5036665F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F656F5D5-BC8B-4362-8583-3E55C246030C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{DD773AE9-4335-4BE7-A63B-9F3DEDF18284}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Number</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>SRK</t>
+  </si>
+  <si>
+    <t>ChargePerSquareFootage</t>
+  </si>
+  <si>
+    <t>Tenant</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBA0FBC-D71D-499D-936B-5D9431E6FC66}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -433,9 +439,10 @@
     <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +455,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -462,8 +472,11 @@
       <c r="D2">
         <v>2954</v>
       </c>
+      <c r="E2">
+        <v>3.25</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -476,8 +489,11 @@
       <c r="D3">
         <v>3104</v>
       </c>
+      <c r="E3">
+        <v>3.25</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -485,10 +501,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>2700</v>
+      </c>
+      <c r="E4">
+        <v>3.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>